<commit_message>
Just double checked the trace table
</commit_message>
<xml_diff>
--- a/docs/Requerimientos y trazabilidad.xlsx
+++ b/docs/Requerimientos y trazabilidad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thetr\Documents\Tercer Semestre\Estructuras\matrix_multiplicationLAB1\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72DA776D-37C2-40D8-9CE9-5F5C824998AC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DECDFA61-7029-4A3E-B409-C787636A3407}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{D01F522C-CD57-4B31-8EB4-CE645565B958}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
   <si>
     <t>Requerimiento</t>
   </si>
@@ -114,6 +114,39 @@
   </si>
   <si>
     <t xml:space="preserve">Se muestra gráficamente el resultado de la multiplicación realizada. </t>
+  </si>
+  <si>
+    <t>initialize()</t>
+  </si>
+  <si>
+    <t>GUIController</t>
+  </si>
+  <si>
+    <t>update()</t>
+  </si>
+  <si>
+    <t>generate(ActionEvent)</t>
+  </si>
+  <si>
+    <t>generateRandomMatrix(int, int, int, int, boolean)</t>
+  </si>
+  <si>
+    <t>BattleBoard</t>
+  </si>
+  <si>
+    <t>fillAndShowMatrix()</t>
+  </si>
+  <si>
+    <t>isRepeated(int, int[][])</t>
+  </si>
+  <si>
+    <t>componetToComponetMultiplier()</t>
+  </si>
+  <si>
+    <t>auxMulti(int, int)</t>
+  </si>
+  <si>
+    <t>multi(int[], int[])</t>
   </si>
 </sst>
 </file>
@@ -283,82 +316,82 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -675,30 +708,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C654AF1-D328-4FCA-9C02-B2147883C250}">
-  <dimension ref="C1:G41"/>
+  <dimension ref="C1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="42.109375" customWidth="1"/>
+    <col min="5" max="5" width="45.5546875" customWidth="1"/>
     <col min="6" max="6" width="28.44140625" customWidth="1"/>
     <col min="7" max="7" width="38.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="23"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="14"/>
     </row>
     <row r="3" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C3" s="3" t="s">
@@ -752,19 +785,19 @@
       </c>
     </row>
     <row r="6" spans="3:7" ht="58.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="9" t="s">
         <v>24</v>
       </c>
     </row>
@@ -784,32 +817,32 @@
       </c>
     </row>
     <row r="8" spans="3:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
     </row>
     <row r="10" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
     </row>
     <row r="11" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
     </row>
     <row r="12" spans="3:7" x14ac:dyDescent="0.3">
       <c r="F12" s="1"/>
@@ -832,156 +865,240 @@
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="25"/>
-      <c r="E18" s="26"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="17"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="20" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="27"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="4"/>
+      <c r="C20" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="21" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C21" s="28"/>
       <c r="D21" s="18"/>
-      <c r="E21" s="6"/>
+      <c r="E21" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="22" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C22" s="29"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="6"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="5" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="23" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C23" s="27"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="4"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="24" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C24" s="28"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="4"/>
+      <c r="C24" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="25" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C25" s="29"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="6"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="26" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C26" s="13"/>
+      <c r="C26" s="28"/>
       <c r="D26" s="18"/>
-      <c r="E26" s="5"/>
+      <c r="E26" s="5" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="27" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C27" s="14"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="4"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="28" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C28" s="13"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="5"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="29" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C29" s="15"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="5"/>
-    </row>
-    <row r="30" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C30" s="14"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="7"/>
-    </row>
-    <row r="31" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C31" s="13"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="5"/>
-    </row>
-    <row r="32" spans="3:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C32" s="14"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="5"/>
-    </row>
-    <row r="33" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="7"/>
-    </row>
-    <row r="34" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="7"/>
-    </row>
-    <row r="35" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C35" s="20"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="7"/>
-    </row>
-    <row r="36" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="7"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="3:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="24"/>
+      <c r="E30" s="27"/>
+    </row>
+    <row r="31" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C31" s="25"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="26"/>
+    </row>
+    <row r="32" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C32" s="25"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="26"/>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C33" s="25"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="27"/>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C34" s="25"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="27"/>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C35" s="25"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="27"/>
+    </row>
+    <row r="36" spans="3:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C36" s="25"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="27"/>
     </row>
     <row r="37" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="7"/>
+      <c r="C37" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="38" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C38" s="13"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="7"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="39" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C39" s="15"/>
+      <c r="C39" s="20"/>
       <c r="D39" s="20"/>
-      <c r="E39" s="7"/>
+      <c r="E39" s="5" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="40" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C40" s="14"/>
+      <c r="C40" s="20"/>
       <c r="D40" s="20"/>
-      <c r="E40" s="7"/>
-    </row>
-    <row r="41" spans="3:5" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+      <c r="E40" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C42" s="20"/>
+      <c r="D42" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C43" s="20"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C44" s="20"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C45" s="20"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="46" spans="3:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C46" s="21"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="47" spans="3:5" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="10">
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="C24:C29"/>
+    <mergeCell ref="C37:C46"/>
+    <mergeCell ref="D37:D41"/>
+    <mergeCell ref="D42:D46"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="D26:D27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>